<commit_message>
arreglado el error del saldo Null
</commit_message>
<xml_diff>
--- a/xls/locales.xlsx
+++ b/xls/locales.xlsx
@@ -1140,8 +1140,8 @@
   </sheetPr>
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1149,7 +1149,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.56"/>
@@ -1256,6 +1256,9 @@
       <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" s="0" t="s">
         <v>22</v>
       </c>
@@ -1361,6 +1364,9 @@
       <c r="G6" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I6" s="0" t="s">
         <v>36</v>
       </c>
@@ -1394,6 +1400,9 @@
       <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I7" s="0" t="s">
         <v>36</v>
       </c>
@@ -1463,6 +1472,9 @@
       <c r="G9" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" s="0" t="s">
         <v>50</v>
       </c>
@@ -1568,6 +1580,9 @@
       <c r="G12" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I12" s="0" t="s">
         <v>67</v>
       </c>
@@ -1781,6 +1796,9 @@
       <c r="G18" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I18" s="0" t="s">
         <v>97</v>
       </c>
@@ -1814,6 +1832,9 @@
       <c r="G19" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I19" s="0" t="s">
         <v>102</v>
       </c>
@@ -1991,6 +2012,9 @@
       <c r="G24" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I24" s="0" t="s">
         <v>131</v>
       </c>
@@ -2024,6 +2048,9 @@
       <c r="G25" s="2" t="s">
         <v>135</v>
       </c>
+      <c r="H25" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" s="0" t="s">
         <v>131</v>
       </c>
@@ -2093,6 +2120,9 @@
       <c r="G27" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I27" s="0" t="s">
         <v>146</v>
       </c>
@@ -2162,6 +2192,9 @@
       <c r="G29" s="2" t="s">
         <v>155</v>
       </c>
+      <c r="H29" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I29" s="0" t="s">
         <v>22</v>
       </c>
@@ -2195,6 +2228,9 @@
       <c r="G30" s="2" t="s">
         <v>157</v>
       </c>
+      <c r="H30" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I30" s="0" t="s">
         <v>22</v>
       </c>
@@ -2444,6 +2480,9 @@
       <c r="G37" s="9" t="s">
         <v>185</v>
       </c>
+      <c r="H37" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I37" s="0" t="s">
         <v>126</v>
       </c>
@@ -2513,6 +2552,9 @@
       <c r="G39" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="H39" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I39" s="0" t="s">
         <v>196</v>
       </c>
@@ -2546,6 +2588,9 @@
       <c r="G40" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="H40" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I40" s="0" t="s">
         <v>201</v>
       </c>
@@ -2615,6 +2660,9 @@
       <c r="G42" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="H42" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I42" s="0" t="s">
         <v>210</v>
       </c>
@@ -2648,6 +2696,9 @@
       <c r="G43" s="2" t="s">
         <v>214</v>
       </c>
+      <c r="H43" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I43" s="0" t="s">
         <v>215</v>
       </c>
@@ -2681,6 +2732,9 @@
       <c r="G44" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="H44" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I44" s="0" t="s">
         <v>218</v>
       </c>
@@ -2714,6 +2768,9 @@
       <c r="G45" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="H45" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I45" s="0" t="s">
         <v>218</v>
       </c>
@@ -2747,6 +2804,9 @@
       <c r="G46" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="H46" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I46" s="0" t="s">
         <v>218</v>
       </c>
@@ -2888,6 +2948,9 @@
       <c r="G50" s="2" t="s">
         <v>242</v>
       </c>
+      <c r="H50" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I50" s="0" t="s">
         <v>243</v>
       </c>
@@ -2957,6 +3020,9 @@
       <c r="G52" s="2" t="s">
         <v>253</v>
       </c>
+      <c r="H52" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I52" s="0" t="s">
         <v>254</v>
       </c>
@@ -2990,6 +3056,9 @@
       <c r="G53" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="H53" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I53" s="0" t="s">
         <v>257</v>
       </c>
@@ -3023,6 +3092,9 @@
       <c r="G54" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="H54" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I54" s="0" t="s">
         <v>257</v>
       </c>
@@ -3056,6 +3128,9 @@
       <c r="G55" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="H55" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I55" s="0" t="s">
         <v>262</v>
       </c>
@@ -3233,6 +3308,9 @@
       <c r="G60" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="H60" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I60" s="0" t="s">
         <v>285</v>
       </c>
@@ -3301,6 +3379,9 @@
       </c>
       <c r="G62" s="2" t="s">
         <v>124</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>291</v>

</xml_diff>